<commit_message>
Update User Stories and Backlog as per meeting
Update User Stories and Backlog as per meeting
</commit_message>
<xml_diff>
--- a/TEAM_SOS_BACKLOG_PLANNING.xlsx
+++ b/TEAM_SOS_BACKLOG_PLANNING.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riccardo.dsilva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Team-SOS-Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Priority</t>
   </si>
@@ -40,6 +40,135 @@
   </si>
   <si>
     <t>Team SOS Backlog</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to login to the application from my mobile/desktop and have it remember my credentials.</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to see all the projects in a dashboard. The projects displayed will be from a project management software like  JIRA, TFS etc or manually set by the admin user.</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to see the projects next up, the projects in progress and the projects completed, any known issues in the dashboard</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to record the start time and end time of the projects</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to undo/redo the times set for the project</t>
+  </si>
+  <si>
+    <t>As an end user, I will NOT be able to add/delete/update any of the projects assigned to me</t>
+  </si>
+  <si>
+    <t>As an end user, I will be having options to edit/update my user profile</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to retrieve my password using 'Forget password' option via email</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to submit my changes to the client or to a central repository</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to track the project time offline and submit these changes when online</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to see a detailed report for all/selected projects</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to see a graphical representation of the projects that I have worked on a daily/weekly/monthly basis</t>
+  </si>
+  <si>
+    <t>As an end user, I will be able to see the time spend on each projects and compare it with the planned hours</t>
+  </si>
+  <si>
+    <t>As an end user, I will be having options to send the report via email</t>
+  </si>
+  <si>
+    <t>As an admin user, I will be able to integrate this app with other project management software like JIRA, TFS, HealthRoster, RosterOn etc</t>
+  </si>
+  <si>
+    <t>As an admin user, I will be able to manage projects(add/edit/update) in case if this is not integrated with any project management software</t>
+  </si>
+  <si>
+    <t>As an admin user, I will be able to manage the users and their project domains</t>
+  </si>
+  <si>
+    <t>As an admin user, I will be able to see a consolidated/individual report of all the users</t>
+  </si>
+  <si>
+    <t>As an admin user, I will able to compare the planned hours against the actual hours</t>
+  </si>
+  <si>
+    <t>As an end user, I want the application to run in the background and be available in the notification drop down list for quick easy access or as a widget I can set on the Home Screen.</t>
+  </si>
+  <si>
+    <t>As an end user, I want the start time of my new task to be automatically populated with the finish time of my previous task or the current time on my mobile device</t>
+  </si>
+  <si>
+    <t>As an end user, I want to be notified if my submitted tasks for the day have been accepted or rejected</t>
+  </si>
+  <si>
+    <t>As an end user, I want to be able to see any tasks that I have entered in my calendar on my mobile device</t>
+  </si>
+  <si>
+    <t>As an end user, I want to be able to download the summary as a PDF onto my mobile device or sent via an email</t>
+  </si>
+  <si>
+    <t>As an end user, I want to be able to download the graph as an Excel/PDF onto my mobile device or sent via an email</t>
+  </si>
+  <si>
+    <t>As a manager, I want to be notified of all task submissions for the day</t>
+  </si>
+  <si>
+    <t>As a manager, I want to be able to Accept any submitted tasks for the day</t>
+  </si>
+  <si>
+    <t>As a manager, I want to be able to Reject any submitted tasks for the day and provide a comment as to why it was rejected</t>
+  </si>
+  <si>
+    <t>As an Admin User Ability to add, modify, and delete high level project details</t>
+  </si>
+  <si>
+    <t>As an Admin User have the Ability to add, modify, and delete resources</t>
+  </si>
+  <si>
+    <t>As an Admin User have the Ability to assign resources to projects</t>
+  </si>
+  <si>
+    <t>As an Admin User have the Ability to assign project tasks to resources</t>
+  </si>
+  <si>
+    <t>As an End User have the Ability to export assigned tasks to resources outlook calendar</t>
+  </si>
+  <si>
+    <t>As an Admin User have the Ability to view what tasks have been assigned to resources</t>
+  </si>
+  <si>
+    <t>Ability to log (create, update, delete) benefits against a Project</t>
+  </si>
+  <si>
+    <t>FUTURE DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>Ability to log (create, update, delete) business requirements against a project, linking the benefits to the business requirements</t>
+  </si>
+  <si>
+    <t>Ability to assign (create, update, delete) functional requirements to business requirements</t>
+  </si>
+  <si>
+    <t>Ability to assign (create, update, delete) non-functional requirements to a Project</t>
+  </si>
+  <si>
+    <t>Ability to assign (create, update, delete) transition requirements to a Project</t>
+  </si>
+  <si>
+    <t>Provide a view providing a complete traceability matrix of project, business requirements, benefits, functional, non functional, transition requirements</t>
+  </si>
+  <si>
+    <t>Provide a view if a business requirement was not going to be done, what would be the impact to the business benefits.</t>
+  </si>
+  <si>
+    <t>As an end user I want the Ability to add, modify, and delete default project tasks</t>
   </si>
 </sst>
 </file>
@@ -63,12 +192,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,13 +230,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -100,7 +254,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -116,8 +270,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:B11" totalsRowShown="0">
-  <autoFilter ref="A4:B11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:B34" totalsRowShown="0">
+  <autoFilter ref="A4:B34"/>
+  <sortState ref="A5:B34">
+    <sortCondition ref="A4:A34"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" name="Priority" dataDxfId="1">
       <calculatedColumnFormula>COUNT(Table1[Priority] + 1)</calculatedColumnFormula>
@@ -404,31 +561,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="73.77734375" customWidth="1"/>
+    <col min="2" max="2" width="155.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -439,16 +597,362 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>2</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>2</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>2</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>2</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C41:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -473,14 +977,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1"/>
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -494,7 +998,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>